<commit_message>
Indicatoren en taalfout in template aangepast
</commit_message>
<xml_diff>
--- a/oko/config oko.xlsx
+++ b/oko/config oko.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/0. Github/report_excel_to_powerpoint/oko/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1028" documentId="13_ncr:1_{BEF9BC84-22C2-4587-9B7D-81FBCE0907AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318B3D23-899D-4958-BA60-D9D6D2476CB3}"/>
+  <xr:revisionPtr revIDLastSave="1032" documentId="13_ncr:1_{BEF9BC84-22C2-4587-9B7D-81FBCE0907AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59DDB5BA-EBC5-4329-B23F-20D999850F75}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
@@ -1192,12 +1192,6 @@
     <t>Rookt niet; Vapet niet</t>
   </si>
   <si>
-    <t>De houding van ouders ten opzichte van hangt samen met het alcoholgebruik van jongeren. Van de jongeren die geen (of alleen een slokje) alcohol drinken geeft LOAGKA319 aan dat hun ouders het goed zouden vinden als ze toch alcohol zouden drinken. Van de jongeren die alcohol drinken geeft LOAGK3A1 aan dat hun ouders alcohol drinken goed vinden.</t>
-  </si>
-  <si>
-    <t>LOAGKA319; LOAGK3A1</t>
-  </si>
-  <si>
     <t>LOAGK3A1; LOAGK3A2; LOAGK3A3; LOAGK3A4; LOAGK3A5; LOAGK3A6; LOAGK3A7; LOAGK3A8; LOAGK3A9; LOAGK3A10</t>
   </si>
   <si>
@@ -1211,6 +1205,12 @@
   </si>
   <si>
     <t>Schoolbeleving</t>
+  </si>
+  <si>
+    <t>LOAGK3A25; LOAGK3A16</t>
+  </si>
+  <si>
+    <t>De houding van ouders ten opzichte van hangt samen met het alcoholgebruik van jongeren. Van de jongeren die geen (of alleen een slokje) alcohol drinken geeft LOAGK3A25 aan dat hun ouders het goed zouden vinden als ze toch alcohol zouden drinken. Van de jongeren die alcohol drinken geeft LOAGK3A16 aan dat hun ouders alcohol drinken goed vinden.</t>
   </si>
 </sst>
 </file>
@@ -1940,9 +1940,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B8C6B-747D-4246-8EF4-E1910EE284AD}">
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C39" sqref="C39"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="20" spans="1:20" ht="51" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>96</v>
@@ -2703,7 +2703,7 @@
         <v>36</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>177</v>
@@ -2741,7 +2741,7 @@
         <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>168</v>
@@ -3256,19 +3256,19 @@
     </row>
     <row r="39" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>160</v>
@@ -4421,6 +4421,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -4434,15 +4443,6 @@
     </TaxKeywordTaxHTField>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4731,6 +4731,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4738,14 +4746,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
     <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fouten in configuratie aangepast
</commit_message>
<xml_diff>
--- a/oko/config oko.xlsx
+++ b/oko/config oko.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/0. Github/report_excel_to_powerpoint/oko/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1123" documentId="13_ncr:1_{BEF9BC84-22C2-4587-9B7D-81FBCE0907AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71915E7E-7480-4148-A079-0C04A6142CED}"/>
+  <xr:revisionPtr revIDLastSave="1133" documentId="13_ncr:1_{BEF9BC84-22C2-4587-9B7D-81FBCE0907AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CC38DC0-B101-4F41-906F-9EC679CF0B09}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5265" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{340DDFAE-1A83-41FC-A379-531A17E4526A}"/>
   </bookViews>
   <sheets>
     <sheet name="reports" sheetId="4" r:id="rId1"/>
@@ -641,7 +641,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="407">
   <si>
     <t>type</t>
   </si>
@@ -1582,9 +1582,6 @@
     <t>1 = (Vaak) tot altijd eenzaam; 1 = (Zeer) vaak gestrest</t>
   </si>
   <si>
-    <t>0 = (Zeer) goede mentale gezondheid; 1 = (Zeer) slechte of gaat wel mentale gezondheid</t>
-  </si>
-  <si>
     <t>Middelengebruik en mentale gezondheid</t>
   </si>
   <si>
@@ -1859,6 +1856,12 @@
   </si>
   <si>
     <t>Middelengebruik en schoolbeleving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOCHK3S7 </t>
+  </si>
+  <si>
+    <t>0 = (Zeer) slechte of gaat wel mentale gezondheid; 1 = (Zeer) goede mentale gezondheid</t>
   </si>
 </sst>
 </file>
@@ -2639,24 +2642,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0AA7A9-459B-4958-BBC2-94F84CFD8846}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="4"/>
+    <col min="3" max="3" width="27.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>235</v>
       </c>
@@ -2717,21 +2720,21 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>235</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>234</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>403</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>404</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>156</v>
@@ -2763,33 +2766,33 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="80.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.88671875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="17" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="2"/>
+    <col min="15" max="15" width="31.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
@@ -2854,7 +2857,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -2877,7 +2880,7 @@
       <c r="P2" s="2"/>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -2899,7 +2902,7 @@
       </c>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -2926,7 +2929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -2955,7 +2958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -2990,7 +2993,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>239</v>
       </c>
@@ -3019,7 +3022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>239</v>
       </c>
@@ -3054,7 +3057,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>161</v>
       </c>
@@ -3083,7 +3086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>161</v>
       </c>
@@ -3118,7 +3121,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>109</v>
       </c>
@@ -3153,7 +3156,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
@@ -3188,7 +3191,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
@@ -3226,7 +3229,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -3261,7 +3264,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>145</v>
       </c>
@@ -3290,7 +3293,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>168</v>
       </c>
@@ -3319,7 +3322,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>169</v>
       </c>
@@ -3348,7 +3351,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>111</v>
       </c>
@@ -3383,7 +3386,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>111</v>
       </c>
@@ -3418,7 +3421,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>261</v>
       </c>
@@ -3447,7 +3450,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>147</v>
       </c>
@@ -3483,7 +3486,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>206</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>59</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
@@ -3595,7 +3598,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>172</v>
       </c>
@@ -3624,7 +3627,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>175</v>
       </c>
@@ -3653,7 +3656,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>67</v>
       </c>
@@ -3688,7 +3691,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
@@ -3723,7 +3726,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>250</v>
       </c>
@@ -3758,7 +3761,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>204</v>
       </c>
@@ -3794,7 +3797,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>205</v>
       </c>
@@ -3830,7 +3833,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>77</v>
       </c>
@@ -3859,7 +3862,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>78</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>105</v>
       </c>
@@ -3932,7 +3935,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>104</v>
       </c>
@@ -3967,7 +3970,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>106</v>
       </c>
@@ -4002,7 +4005,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>239</v>
       </c>
@@ -4040,7 +4043,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>148</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>259</v>
       </c>
@@ -4113,7 +4116,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>80</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>125</v>
       </c>
@@ -4171,7 +4174,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>240</v>
       </c>
@@ -4200,7 +4203,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>241</v>
       </c>
@@ -4229,7 +4232,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>125</v>
       </c>
@@ -4264,7 +4267,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>242</v>
       </c>
@@ -4299,7 +4302,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>141</v>
       </c>
@@ -4343,7 +4346,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>141</v>
       </c>
@@ -4360,7 +4363,7 @@
         <v>149</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>212</v>
+        <v>405</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>214</v>
@@ -4387,7 +4390,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>87</v>
       </c>
@@ -4416,7 +4419,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>126</v>
       </c>
@@ -4451,7 +4454,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>127</v>
       </c>
@@ -4484,7 +4487,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>127</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="69" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>145</v>
       </c>
@@ -4557,7 +4560,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>123</v>
       </c>
@@ -4595,7 +4598,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>192</v>
       </c>
@@ -4633,7 +4636,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>189</v>
       </c>
@@ -4671,7 +4674,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
@@ -4709,7 +4712,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>243</v>
       </c>
@@ -4744,7 +4747,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>146</v>
       </c>
@@ -4782,7 +4785,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>239</v>
       </c>
@@ -4820,7 +4823,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>128</v>
       </c>
@@ -4855,7 +4858,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>93</v>
       </c>
@@ -4890,7 +4893,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>94</v>
       </c>
@@ -4919,7 +4922,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>95</v>
       </c>
@@ -4948,7 +4951,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>184</v>
       </c>
@@ -4977,7 +4980,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>183</v>
       </c>
@@ -5006,7 +5009,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>150</v>
       </c>
@@ -5041,7 +5044,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>112</v>
       </c>
@@ -5076,7 +5079,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>143</v>
       </c>
@@ -5114,7 +5117,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>144</v>
       </c>
@@ -5143,7 +5146,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="51" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>145</v>
       </c>
@@ -5181,7 +5184,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="51" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>239</v>
       </c>
@@ -5251,38 +5254,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BEB4C1-A925-4FAE-9007-19794D9EEA69}">
   <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="73.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="17" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="3" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="31.28515625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.5546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="31.33203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="47.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.85546875" style="2"/>
+    <col min="20" max="20" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="47.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
@@ -5350,7 +5351,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>276</v>
       </c>
@@ -5367,7 +5368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>279</v>
       </c>
@@ -5384,7 +5385,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>282</v>
       </c>
@@ -5419,7 +5420,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>282</v>
       </c>
@@ -5457,7 +5458,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>286</v>
       </c>
@@ -5504,7 +5505,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>292</v>
       </c>
@@ -5551,7 +5552,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>296</v>
       </c>
@@ -5586,7 +5587,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>296</v>
       </c>
@@ -5624,7 +5625,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>297</v>
       </c>
@@ -5671,7 +5672,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>299</v>
       </c>
@@ -5718,7 +5719,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>302</v>
       </c>
@@ -5753,7 +5754,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>302</v>
       </c>
@@ -5791,7 +5792,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>303</v>
       </c>
@@ -5838,7 +5839,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>305</v>
       </c>
@@ -5885,7 +5886,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>308</v>
       </c>
@@ -5921,7 +5922,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>308</v>
       </c>
@@ -5959,7 +5960,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>310</v>
       </c>
@@ -5979,7 +5980,7 @@
         <v>252</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>313</v>
+        <v>406</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>156</v>
@@ -6006,27 +6007,27 @@
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>314</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>315</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>252</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>313</v>
+        <v>406</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>156</v>
@@ -6053,15 +6054,15 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>317</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>318</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>34</v>
@@ -6088,15 +6089,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>317</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>318</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>34</v>
@@ -6126,27 +6127,27 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>319</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>322</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>156</v>
@@ -6173,27 +6174,27 @@
         <v>291</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>156</v>
@@ -6220,9 +6221,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>36</v>
@@ -6255,9 +6256,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>36</v>
@@ -6293,27 +6294,27 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>325</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>326</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>96</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>156</v>
@@ -6340,27 +6341,27 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>156</v>
@@ -6387,9 +6388,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>36</v>
@@ -6413,7 +6414,7 @@
         <v>9</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>284</v>
@@ -6422,12 +6423,12 @@
         <v>103</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>36</v>
@@ -6454,7 +6455,7 @@
         <v>9</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>285</v>
@@ -6463,12 +6464,12 @@
         <v>103</v>
       </c>
       <c r="V29" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>333</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>36</v>
@@ -6486,7 +6487,7 @@
         <v>225</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>156</v>
@@ -6501,7 +6502,7 @@
         <v>9</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>290</v>
@@ -6513,30 +6514,30 @@
         <v>291</v>
       </c>
       <c r="V30" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>336</v>
-      </c>
       <c r="B31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>225</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>156</v>
@@ -6551,7 +6552,7 @@
         <v>9</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>295</v>
@@ -6563,12 +6564,12 @@
         <v>291</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>36</v>
@@ -6592,7 +6593,7 @@
         <v>10</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P32" s="2" t="s">
         <v>284</v>
@@ -6601,12 +6602,12 @@
         <v>103</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>36</v>
@@ -6633,7 +6634,7 @@
         <v>10</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P33" s="2" t="s">
         <v>285</v>
@@ -6642,12 +6643,12 @@
         <v>103</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>36</v>
@@ -6665,7 +6666,7 @@
         <v>223</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>156</v>
@@ -6680,7 +6681,7 @@
         <v>10</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P34" s="2" t="s">
         <v>290</v>
@@ -6692,30 +6693,30 @@
         <v>291</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>156</v>
@@ -6730,7 +6731,7 @@
         <v>10</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P35" s="2" t="s">
         <v>295</v>
@@ -6742,12 +6743,12 @@
         <v>291</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>36</v>
@@ -6771,7 +6772,7 @@
         <v>11</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P36" s="2" t="s">
         <v>284</v>
@@ -6780,12 +6781,12 @@
         <v>103</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>36</v>
@@ -6812,7 +6813,7 @@
         <v>11</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>285</v>
@@ -6821,12 +6822,12 @@
         <v>103</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>36</v>
@@ -6844,7 +6845,7 @@
         <v>224</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>156</v>
@@ -6859,7 +6860,7 @@
         <v>11</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P38" s="2" t="s">
         <v>290</v>
@@ -6871,30 +6872,30 @@
         <v>291</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>224</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>156</v>
@@ -6909,7 +6910,7 @@
         <v>11</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P39" s="2" t="s">
         <v>295</v>
@@ -6921,18 +6922,18 @@
         <v>291</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>34</v>
@@ -6950,7 +6951,7 @@
         <v>12</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P40" s="2" t="s">
         <v>284</v>
@@ -6959,18 +6960,18 @@
         <v>103</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>34</v>
@@ -6991,7 +6992,7 @@
         <v>12</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P41" s="2" t="s">
         <v>285</v>
@@ -7000,12 +7001,12 @@
         <v>103</v>
       </c>
       <c r="V41" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="21" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
-        <v>349</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>36</v>
@@ -7020,10 +7021,10 @@
         <v>288</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>156</v>
@@ -7038,7 +7039,7 @@
         <v>12</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P42" s="2" t="s">
         <v>290</v>
@@ -7050,30 +7051,30 @@
         <v>291</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>156</v>
@@ -7088,7 +7089,7 @@
         <v>12</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P43" s="2" t="s">
         <v>295</v>
@@ -7100,18 +7101,18 @@
         <v>291</v>
       </c>
       <c r="V43" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A44" s="22" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
+      <c r="B44" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>34</v>
@@ -7129,7 +7130,7 @@
         <v>13</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P44" s="2" t="s">
         <v>284</v>
@@ -7138,18 +7139,18 @@
         <v>103</v>
       </c>
       <c r="V44" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>34</v>
@@ -7170,7 +7171,7 @@
         <v>13</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P45" s="2" t="s">
         <v>285</v>
@@ -7179,12 +7180,12 @@
         <v>103</v>
       </c>
       <c r="V45" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>36</v>
@@ -7199,10 +7200,10 @@
         <v>288</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>156</v>
@@ -7217,7 +7218,7 @@
         <v>13</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P46" s="2" t="s">
         <v>290</v>
@@ -7229,30 +7230,30 @@
         <v>291</v>
       </c>
       <c r="V46" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A47" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>156</v>
@@ -7267,7 +7268,7 @@
         <v>13</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P47" s="2" t="s">
         <v>295</v>
@@ -7279,18 +7280,18 @@
         <v>291</v>
       </c>
       <c r="V47" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>34</v>
@@ -7308,7 +7309,7 @@
         <v>14</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P48" s="2" t="s">
         <v>284</v>
@@ -7317,18 +7318,18 @@
         <v>103</v>
       </c>
       <c r="V48" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>34</v>
@@ -7349,7 +7350,7 @@
         <v>14</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P49" s="2" t="s">
         <v>285</v>
@@ -7358,12 +7359,12 @@
         <v>103</v>
       </c>
       <c r="V49" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>360</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>361</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>36</v>
@@ -7378,10 +7379,10 @@
         <v>288</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>156</v>
@@ -7396,7 +7397,7 @@
         <v>14</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P50" s="2" t="s">
         <v>290</v>
@@ -7408,30 +7409,30 @@
         <v>291</v>
       </c>
       <c r="V50" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>364</v>
-      </c>
       <c r="B51" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>156</v>
@@ -7446,7 +7447,7 @@
         <v>14</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P51" s="2" t="s">
         <v>295</v>
@@ -7458,12 +7459,12 @@
         <v>291</v>
       </c>
       <c r="V51" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>36</v>
@@ -7487,7 +7488,7 @@
         <v>15</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>284</v>
@@ -7496,12 +7497,12 @@
         <v>103</v>
       </c>
       <c r="V52" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>36</v>
@@ -7528,7 +7529,7 @@
         <v>15</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>285</v>
@@ -7537,12 +7538,12 @@
         <v>103</v>
       </c>
       <c r="V53" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>36</v>
@@ -7560,7 +7561,7 @@
         <v>212</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>156</v>
@@ -7575,7 +7576,7 @@
         <v>15</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P54" s="2" t="s">
         <v>290</v>
@@ -7587,30 +7588,30 @@
         <v>291</v>
       </c>
       <c r="V54" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>212</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>156</v>
@@ -7625,7 +7626,7 @@
         <v>15</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P55" s="2" t="s">
         <v>295</v>
@@ -7637,18 +7638,18 @@
         <v>291</v>
       </c>
       <c r="V55" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>34</v>
@@ -7666,7 +7667,7 @@
         <v>16</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P56" s="2" t="s">
         <v>284</v>
@@ -7675,18 +7676,18 @@
         <v>103</v>
       </c>
       <c r="V56" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>34</v>
@@ -7707,7 +7708,7 @@
         <v>16</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P57" s="2" t="s">
         <v>285</v>
@@ -7716,12 +7717,12 @@
         <v>103</v>
       </c>
       <c r="V57" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22" ht="63.75" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" ht="69" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>36</v>
@@ -7736,10 +7737,10 @@
         <v>288</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>156</v>
@@ -7754,7 +7755,7 @@
         <v>16</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P58" s="2" t="s">
         <v>290</v>
@@ -7766,30 +7767,30 @@
         <v>291</v>
       </c>
       <c r="V58" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="59" spans="1:22" ht="63.75" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="69" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>156</v>
@@ -7804,7 +7805,7 @@
         <v>16</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P59" s="2" t="s">
         <v>295</v>
@@ -7816,12 +7817,12 @@
         <v>291</v>
       </c>
       <c r="V59" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>36</v>
@@ -7845,7 +7846,7 @@
         <v>17</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P60" s="2" t="s">
         <v>284</v>
@@ -7854,12 +7855,12 @@
         <v>103</v>
       </c>
       <c r="V60" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>36</v>
@@ -7886,7 +7887,7 @@
         <v>17</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P61" s="2" t="s">
         <v>285</v>
@@ -7895,12 +7896,12 @@
         <v>103</v>
       </c>
       <c r="V61" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="20" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
-        <v>377</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>36</v>
@@ -7918,7 +7919,7 @@
         <v>220</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>156</v>
@@ -7933,7 +7934,7 @@
         <v>17</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P62" s="2" t="s">
         <v>290</v>
@@ -7945,30 +7946,30 @@
         <v>291</v>
       </c>
       <c r="V62" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>380</v>
-      </c>
       <c r="B63" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>220</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>156</v>
@@ -7983,7 +7984,7 @@
         <v>17</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P63" s="2" t="s">
         <v>295</v>
@@ -7995,18 +7996,18 @@
         <v>291</v>
       </c>
       <c r="V63" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C64" s="23" t="s">
-        <v>382</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>34</v>
@@ -8024,7 +8025,7 @@
         <v>18</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P64" s="2" t="s">
         <v>284</v>
@@ -8033,18 +8034,18 @@
         <v>103</v>
       </c>
       <c r="V64" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C65" s="23" t="s">
-        <v>382</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>34</v>
@@ -8065,7 +8066,7 @@
         <v>18</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P65" s="2" t="s">
         <v>285</v>
@@ -8074,12 +8075,12 @@
         <v>103</v>
       </c>
       <c r="V65" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
         <v>376</v>
-      </c>
-    </row>
-    <row r="66" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
-        <v>377</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>36</v>
@@ -8094,10 +8095,10 @@
         <v>288</v>
       </c>
       <c r="F66" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>383</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>156</v>
@@ -8112,7 +8113,7 @@
         <v>18</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P66" s="2" t="s">
         <v>290</v>
@@ -8124,30 +8125,30 @@
         <v>291</v>
       </c>
       <c r="V66" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
-        <v>380</v>
-      </c>
       <c r="B67" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G67" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>383</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>156</v>
@@ -8162,7 +8163,7 @@
         <v>18</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P67" s="2" t="s">
         <v>295</v>
@@ -8174,18 +8175,18 @@
         <v>291</v>
       </c>
       <c r="V67" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="68" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" s="23" t="s">
         <v>384</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>385</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>34</v>
@@ -8203,7 +8204,7 @@
         <v>19</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P68" s="2" t="s">
         <v>284</v>
@@ -8212,18 +8213,18 @@
         <v>103</v>
       </c>
       <c r="V68" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" s="23" t="s">
         <v>384</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>385</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>34</v>
@@ -8244,7 +8245,7 @@
         <v>19</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P69" s="2" t="s">
         <v>285</v>
@@ -8253,12 +8254,12 @@
         <v>103</v>
       </c>
       <c r="V69" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="70" spans="1:22" ht="51" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>36</v>
@@ -8273,10 +8274,10 @@
         <v>288</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>156</v>
@@ -8291,7 +8292,7 @@
         <v>19</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P70" s="2" t="s">
         <v>290</v>
@@ -8303,30 +8304,30 @@
         <v>291</v>
       </c>
       <c r="V70" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22" ht="51" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>156</v>
@@ -8341,7 +8342,7 @@
         <v>19</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P71" s="2" t="s">
         <v>295</v>
@@ -8353,18 +8354,18 @@
         <v>291</v>
       </c>
       <c r="V71" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" s="23" t="s">
         <v>389</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C72" s="23" t="s">
-        <v>390</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>34</v>
@@ -8382,7 +8383,7 @@
         <v>20</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P72" s="2" t="s">
         <v>284</v>
@@ -8391,18 +8392,18 @@
         <v>103</v>
       </c>
       <c r="V72" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="73" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" s="23" t="s">
         <v>389</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C73" s="23" t="s">
-        <v>390</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>34</v>
@@ -8423,7 +8424,7 @@
         <v>20</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P73" s="2" t="s">
         <v>285</v>
@@ -8432,12 +8433,12 @@
         <v>103</v>
       </c>
       <c r="V73" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22" ht="51" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A74" s="20" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>36</v>
@@ -8452,10 +8453,10 @@
         <v>288</v>
       </c>
       <c r="F74" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G74" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>156</v>
@@ -8470,7 +8471,7 @@
         <v>20</v>
       </c>
       <c r="O74" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P74" s="2" t="s">
         <v>290</v>
@@ -8482,30 +8483,30 @@
         <v>291</v>
       </c>
       <c r="V74" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="75" spans="1:22" ht="51" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F75" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>156</v>
@@ -8520,7 +8521,7 @@
         <v>20</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P75" s="2" t="s">
         <v>295</v>
@@ -8532,12 +8533,12 @@
         <v>291</v>
       </c>
       <c r="V75" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>36</v>
@@ -8561,7 +8562,7 @@
         <v>21</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P76" s="2" t="s">
         <v>284</v>
@@ -8570,12 +8571,12 @@
         <v>103</v>
       </c>
       <c r="V76" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>36</v>
@@ -8602,7 +8603,7 @@
         <v>21</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P77" s="2" t="s">
         <v>285</v>
@@ -8611,12 +8612,12 @@
         <v>103</v>
       </c>
       <c r="V77" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A78" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>36</v>
@@ -8634,7 +8635,7 @@
         <v>221</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>156</v>
@@ -8649,7 +8650,7 @@
         <v>21</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P78" s="2" t="s">
         <v>290</v>
@@ -8661,30 +8662,30 @@
         <v>291</v>
       </c>
       <c r="V78" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="79" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A79" s="20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D79" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>221</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>156</v>
@@ -8699,7 +8700,7 @@
         <v>21</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P79" s="2" t="s">
         <v>295</v>
@@ -8711,18 +8712,18 @@
         <v>291</v>
       </c>
       <c r="V79" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C80" s="23" t="s">
         <v>396</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C80" s="23" t="s">
-        <v>397</v>
       </c>
       <c r="D80" s="18" t="s">
         <v>34</v>
@@ -8740,7 +8741,7 @@
         <v>22</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P80" s="2" t="s">
         <v>284</v>
@@ -8749,18 +8750,18 @@
         <v>103</v>
       </c>
       <c r="V80" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A81" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C81" s="23" t="s">
         <v>396</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C81" s="23" t="s">
-        <v>397</v>
       </c>
       <c r="D81" s="18" t="s">
         <v>34</v>
@@ -8781,7 +8782,7 @@
         <v>22</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P81" s="2" t="s">
         <v>285</v>
@@ -8790,12 +8791,12 @@
         <v>103</v>
       </c>
       <c r="V81" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A82" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>36</v>
@@ -8810,10 +8811,10 @@
         <v>288</v>
       </c>
       <c r="F82" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G82" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>156</v>
@@ -8828,7 +8829,7 @@
         <v>22</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P82" s="2" t="s">
         <v>290</v>
@@ -8840,30 +8841,30 @@
         <v>291</v>
       </c>
       <c r="V82" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="83" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A83" s="20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D83" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F83" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G83" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>156</v>
@@ -8878,7 +8879,7 @@
         <v>22</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P83" s="2" t="s">
         <v>295</v>
@@ -8890,18 +8891,18 @@
         <v>291</v>
       </c>
       <c r="V83" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A84" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C84" s="23" t="s">
         <v>399</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C84" s="23" t="s">
-        <v>400</v>
       </c>
       <c r="D84" s="18" t="s">
         <v>34</v>
@@ -8919,7 +8920,7 @@
         <v>23</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P84" s="2" t="s">
         <v>284</v>
@@ -8928,18 +8929,18 @@
         <v>103</v>
       </c>
       <c r="V84" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A85" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C85" s="23" t="s">
         <v>399</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C85" s="23" t="s">
-        <v>400</v>
       </c>
       <c r="D85" s="18" t="s">
         <v>34</v>
@@ -8960,7 +8961,7 @@
         <v>23</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P85" s="2" t="s">
         <v>285</v>
@@ -8969,12 +8970,12 @@
         <v>103</v>
       </c>
       <c r="V85" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="86" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A86" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>36</v>
@@ -8989,10 +8990,10 @@
         <v>288</v>
       </c>
       <c r="F86" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G86" s="3" t="s">
         <v>400</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>401</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>156</v>
@@ -9007,7 +9008,7 @@
         <v>23</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P86" s="2" t="s">
         <v>290</v>
@@ -9019,30 +9020,30 @@
         <v>291</v>
       </c>
       <c r="V86" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="87" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A87" s="20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D87" s="18" t="s">
         <v>98</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F87" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>400</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>401</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>156</v>
@@ -9057,7 +9058,7 @@
         <v>23</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P87" s="2" t="s">
         <v>295</v>
@@ -9069,7 +9070,7 @@
         <v>291</v>
       </c>
       <c r="V87" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -9091,29 +9092,14 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e49181b65574406c5282aee675d2d615">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc6d884b6a76c93e77d17ea8b02330de" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="586e6f9b10cb27d3f03483507ae7cb9d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f29125cba2118f3064d103e6e0ba85ce" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="4e95bed8-6d15-4403-ad70-a53422338dca"/>
     <xsd:import namespace="10d3344f-2d16-43d9-a145-97142f5cb288"/>
@@ -9396,7 +9382,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9405,20 +9391,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
-    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7DC8098-0BCF-4335-855B-B63F1C44D88B}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15B2EAB0-CF1E-4BFF-A0B2-760E3129F1CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -9438,10 +9428,22 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EF40A6-8528-4994-A94E-1AE934020AF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFBB421F-7112-4B85-A662-9379706C03DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>